<commit_message>
Cierre 001 añadido - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/09_Cierre/Cierre_001.xlsx
+++ b/ControlCambios/09_Cierre/Cierre_001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\09_Cierre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B679D2B-3B80-4177-9E32-34A2D7F0CC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8D5453-CBC6-4FAD-9EB1-F3C4E26F770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{98812C98-FD81-47D6-8E71-6F0D9EDDF80A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{98812C98-FD81-47D6-8E71-6F0D9EDDF80A}"/>
   </bookViews>
   <sheets>
     <sheet name="Cierre" sheetId="1" r:id="rId1"/>
@@ -59,34 +59,19 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Nombre completo del responsable]</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Correo electrónico del responsable]</t>
-  </si>
-  <si>
     <t>ID del empleado</t>
   </si>
   <si>
-    <t>[Número de empleado asignado al responsable]</t>
-  </si>
-  <si>
     <t>Resumen del cambio</t>
   </si>
   <si>
     <t>Objetivos iniciales</t>
   </si>
   <si>
-    <t xml:space="preserve">[Descripción de los objetivos iniciales del proyecto] </t>
-  </si>
-  <si>
     <t>Cambios implementados</t>
-  </si>
-  <si>
-    <t>[Lista de cambios realizados]</t>
   </si>
   <si>
     <t>Evaluación del cambio</t>
@@ -111,26 +96,41 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">[Éxito / Parcialmente exitoso / Fracaso] </t>
-  </si>
-  <si>
     <t>Aspectos destacados</t>
   </si>
   <si>
-    <t xml:space="preserve">[Logros y aspectos positivos del cambio] </t>
-  </si>
-  <si>
     <t>CIERRE</t>
   </si>
   <si>
     <t>1/1</t>
+  </si>
+  <si>
+    <t>Nicolás Barcia Quintela</t>
+  </si>
+  <si>
+    <t>nicolas.barcia@rai.usc.es</t>
+  </si>
+  <si>
+    <t>NBQ_050100</t>
+  </si>
+  <si>
+    <t>Implementar una funcionalidad de exportación a PDF para resumir las operaciones dentro de un grupo de gasto.</t>
+  </si>
+  <si>
+    <t>Funcionalidad implementada con éxito, incluyendo las medidas de seguridad y protección de datos respectivas.</t>
+  </si>
+  <si>
+    <t>Éxito</t>
+  </si>
+  <si>
+    <t>Se ha conseguido implementar la funcionalidad sin detectar problemas al respecto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,8 +623,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -632,32 +641,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -674,60 +659,76 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="2" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="17" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -737,111 +738,120 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="17" fillId="2" borderId="31" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="17" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -858,9 +868,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -898,7 +908,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1004,7 +1014,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1146,7 +1156,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1157,15 +1167,15 @@
   <dimension ref="D3:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="G24" sqref="G24:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="4:11" ht="15" thickBot="1"/>
     <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">
         <v>0</v>
@@ -1180,312 +1190,325 @@
         <v>2</v>
       </c>
       <c r="J4" s="5">
-        <v>45323</v>
+        <v>45349</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D5" s="7" t="s">
+    <row r="5" spans="4:11" ht="15" thickBot="1">
+      <c r="D5" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="64"/>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="18"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25" t="s">
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="4:11">
+      <c r="D10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="4:11">
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31" t="s">
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
-    </row>
-    <row r="11" spans="4:11">
-      <c r="D11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="34"/>
-    </row>
-    <row r="12" spans="4:11">
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
-    </row>
-    <row r="13" spans="4:11">
-      <c r="D13" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="14" spans="4:11">
-      <c r="D14" s="43"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="10"/>
     </row>
     <row r="15" spans="4:11" ht="15" customHeight="1">
       <c r="D15" s="45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="47"/>
-      <c r="G15" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="18"/>
+      <c r="G15" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="4:11">
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="18"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="4:11">
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="18"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="4:11" ht="15" customHeight="1">
       <c r="D18" s="45" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="47"/>
-      <c r="G18" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="18"/>
+      <c r="G18" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="4:11">
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="18"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="10"/>
     </row>
     <row r="20" spans="4:11">
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="18"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
     </row>
     <row r="21" spans="4:11">
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="63"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="4:11" ht="15" customHeight="1">
-      <c r="D22" s="64" t="s">
-        <v>17</v>
+      <c r="D22" s="48" t="s">
+        <v>12</v>
       </c>
       <c r="E22" s="46"/>
       <c r="F22" s="46"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="18"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="4:11">
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="18"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="10"/>
     </row>
     <row r="24" spans="4:11" ht="15" customHeight="1">
-      <c r="D24" s="67" t="s">
-        <v>18</v>
+      <c r="D24" s="49" t="s">
+        <v>13</v>
       </c>
       <c r="E24" s="46"/>
       <c r="F24" s="47"/>
-      <c r="G24" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="18"/>
+      <c r="G24" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="10"/>
     </row>
     <row r="25" spans="4:11">
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="18"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="10"/>
     </row>
     <row r="26" spans="4:11">
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="18"/>
-    </row>
-    <row r="27" spans="4:11" ht="15.75">
-      <c r="D27" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="75"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="18"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="4:11" ht="15.6">
+      <c r="D27" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="39"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="4:11">
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="18"/>
-    </row>
-    <row r="29" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D29" s="77"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="80"/>
-    </row>
-    <row r="30" spans="4:11" ht="15.75" thickBot="1">
-      <c r="D30" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="82"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="84"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="4:11" ht="15" thickBot="1">
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="37"/>
+    </row>
+    <row r="30" spans="4:11" ht="15" thickBot="1">
+      <c r="D30" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:J13"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:J28"/>
     <mergeCell ref="D30:I30"/>
@@ -1497,20 +1520,10 @@
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:J25"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:J9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G10" r:id="rId1" xr:uid="{75A48E6C-1020-4C13-A7C5-457BC8A38281}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>